<commit_message>
Complete HappyMemory (funciton 2)
</commit_message>
<xml_diff>
--- a/Database/Anxiety_Table.xlsx
+++ b/Database/Anxiety_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\孙博弈\Desktop\SHE Innovates\The-Anxiety-Time-Machine\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA162DCA-95C9-46B7-9898-C68E1CB6674C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738B38C3-9301-4E2A-A823-0F461A32CC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,12 +566,13 @@
   </sheetPr>
   <dimension ref="A1:AA1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="5" max="5" width="23.86328125" customWidth="1"/>
     <col min="6" max="6" width="72.86328125" customWidth="1"/>
     <col min="7" max="7" width="23.265625" customWidth="1"/>
   </cols>

</xml_diff>